<commit_message>
wip: hacking bug with excelize date handling
</commit_message>
<xml_diff>
--- a/drivers/xlsx/testdata/test_datetime.xlsx
+++ b/drivers/xlsx/testdata/test_datetime.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460A590D-1ADF-CB4E-95A5-E78F4F7A419F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5CFD98-88D1-AC40-9B8A-80EDEA759BCF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72000" yWindow="12340" windowWidth="41340" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="76920" yWindow="16120" windowWidth="41340" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>col_datetime</t>
   </si>
@@ -72,16 +72,44 @@
   </si>
   <si>
     <t>7:15pm</t>
+  </si>
+  <si>
+    <t>my_bool</t>
+  </si>
+  <si>
+    <t>A1__</t>
+  </si>
+  <si>
+    <t>A2__</t>
+  </si>
+  <si>
+    <t>A3__</t>
+  </si>
+  <si>
+    <t>A4__</t>
+  </si>
+  <si>
+    <t>G1__</t>
+  </si>
+  <si>
+    <t>G2__</t>
+  </si>
+  <si>
+    <t>G3__</t>
+  </si>
+  <si>
+    <t>G4__</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -117,16 +145,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,141 +431,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G7"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20" customWidth="1"/>
-    <col min="3" max="4" width="12" customWidth="1"/>
-    <col min="5" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="27.33203125" customWidth="1"/>
-    <col min="13" max="13" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="5" width="12" customWidth="1"/>
+    <col min="6" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" customWidth="1"/>
+    <col min="15" max="15" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="9">
         <v>32821</v>
       </c>
-      <c r="B2" s="2">
-        <v>32821</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>32821</v>
       </c>
       <c r="D2" s="3">
         <v>32821</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
+        <v>32821</v>
+      </c>
+      <c r="F2" s="5">
         <v>0</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="4">
         <v>0</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4">
+      <c r="J2" s="4">
         <v>0.80216435185185186</v>
       </c>
-      <c r="I2" s="7">
+      <c r="K2" s="7">
         <v>0.80208333333333337</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>17</v>
-      </c>
-      <c r="K2" s="8">
-        <v>0.80208333333333337</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
       </c>
       <c r="M2" s="8">
         <v>0.80208333333333337</v>
       </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="8">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="9">
         <v>42923.2966087963</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C3" s="2">
         <v>42923.2966087963</v>
-      </c>
-      <c r="C3" s="3">
-        <v>42923</v>
       </c>
       <c r="D3" s="3">
         <v>42923</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
+        <v>42923</v>
+      </c>
+      <c r="F3" s="5">
         <v>0.29660879629955161</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="4">
         <v>0.29660879629955161</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="Q3" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="9">
         <v>42923.2966087963</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>42923</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>0.29660879629955161</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>